<commit_message>
Fixed bug in Excel output not being udpated to reflect manually-added blobs
</commit_message>
<xml_diff>
--- a/Arginine CLS with pH BLOB_DETECTOR.xlsx
+++ b/Arginine CLS with pH BLOB_DETECTOR.xlsx
@@ -111,7 +111,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -338,15 +338,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="0"/>
       </bottom>
@@ -396,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -525,37 +516,30 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,7 +821,7 @@
   <dimension ref="A1:AO37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E3" sqref="E3:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -862,12 +846,12 @@
           <t>Strain</t>
         </is>
       </c>
-      <c r="C1" s="60" t="inlineStr">
+      <c r="C1" s="57" t="inlineStr">
         <is>
           <t>Sample Number</t>
         </is>
       </c>
-      <c r="D1" s="61" t="inlineStr">
+      <c r="D1" s="59" t="inlineStr">
         <is>
           <t>Baseline</t>
         </is>
@@ -938,8 +922,8 @@
       <c r="AN1" s="42" t="n"/>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="41">
-      <c r="A2" s="62" t="n"/>
-      <c r="C2" s="56" t="n"/>
+      <c r="A2" s="50" t="n"/>
+      <c r="C2" s="58" t="n"/>
       <c r="D2" s="42" t="n"/>
       <c r="E2" s="1" t="inlineStr">
         <is>
@@ -1123,7 +1107,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="41">
-      <c r="A3" s="58" t="inlineStr">
+      <c r="A3" s="55" t="inlineStr">
         <is>
           <t>0 mM Arginine</t>
         </is>
@@ -1141,7 +1125,7 @@
         <v/>
       </c>
       <c r="E3" s="9" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F3" s="10" t="inlineStr">
         <is>
@@ -1264,8 +1248,8 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="41">
-      <c r="A4" s="62" t="n"/>
-      <c r="C4" s="55" t="n">
+      <c r="A4" s="50" t="n"/>
+      <c r="C4" s="15" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="16">
@@ -1396,8 +1380,8 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="41">
-      <c r="A5" s="62" t="n"/>
-      <c r="C5" s="55" t="n">
+      <c r="A5" s="50" t="n"/>
+      <c r="C5" s="15" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="16">
@@ -1528,7 +1512,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="41">
-      <c r="A6" s="62" t="n"/>
+      <c r="A6" s="50" t="n"/>
       <c r="B6" s="46" t="n"/>
       <c r="C6" s="23" t="n">
         <v>4</v>
@@ -1661,7 +1645,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="41">
-      <c r="A7" s="62" t="n"/>
+      <c r="A7" s="50" t="n"/>
       <c r="B7" s="47" t="inlineStr">
         <is>
           <t>JS1582</t>
@@ -1798,8 +1782,8 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="41">
-      <c r="A8" s="62" t="n"/>
-      <c r="C8" s="55" t="n">
+      <c r="A8" s="50" t="n"/>
+      <c r="C8" s="15" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="16">
@@ -1930,8 +1914,8 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="41">
-      <c r="A9" s="62" t="n"/>
-      <c r="C9" s="55" t="n">
+      <c r="A9" s="50" t="n"/>
+      <c r="C9" s="15" t="n">
         <v>7</v>
       </c>
       <c r="D9" s="16">
@@ -2062,7 +2046,7 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="41">
-      <c r="A10" s="62" t="n"/>
+      <c r="A10" s="50" t="n"/>
       <c r="B10" s="46" t="n"/>
       <c r="C10" s="23" t="n">
         <v>8</v>
@@ -2195,7 +2179,7 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="41">
-      <c r="A11" s="62" t="n"/>
+      <c r="A11" s="50" t="n"/>
       <c r="B11" s="48" t="inlineStr">
         <is>
           <t>JS1783</t>
@@ -2332,8 +2316,8 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="41">
-      <c r="A12" s="62" t="n"/>
-      <c r="C12" s="55" t="n">
+      <c r="A12" s="50" t="n"/>
+      <c r="C12" s="15" t="n">
         <v>10</v>
       </c>
       <c r="D12" s="16">
@@ -2464,8 +2448,8 @@
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="41">
-      <c r="A13" s="62" t="n"/>
-      <c r="C13" s="55" t="n">
+      <c r="A13" s="50" t="n"/>
+      <c r="C13" s="15" t="n">
         <v>11</v>
       </c>
       <c r="D13" s="16">
@@ -2596,7 +2580,7 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="41">
-      <c r="A14" s="62" t="n"/>
+      <c r="A14" s="50" t="n"/>
       <c r="B14" s="46" t="n"/>
       <c r="C14" s="23" t="n">
         <v>12</v>
@@ -2729,8 +2713,8 @@
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="41">
-      <c r="A15" s="62" t="n"/>
-      <c r="B15" s="59" t="inlineStr">
+      <c r="A15" s="50" t="n"/>
+      <c r="B15" s="56" t="inlineStr">
         <is>
           <t>JS1787</t>
         </is>
@@ -2866,8 +2850,8 @@
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="41">
-      <c r="A16" s="62" t="n"/>
-      <c r="C16" s="55" t="n">
+      <c r="A16" s="50" t="n"/>
+      <c r="C16" s="15" t="n">
         <v>14</v>
       </c>
       <c r="D16" s="16">
@@ -2998,8 +2982,8 @@
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="41">
-      <c r="A17" s="62" t="n"/>
-      <c r="C17" s="55" t="n">
+      <c r="A17" s="50" t="n"/>
+      <c r="C17" s="15" t="n">
         <v>15</v>
       </c>
       <c r="D17" s="16">
@@ -3130,8 +3114,8 @@
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="41">
-      <c r="A18" s="62" t="n"/>
-      <c r="C18" s="55" t="n">
+      <c r="A18" s="50" t="n"/>
+      <c r="C18" s="15" t="n">
         <v>16</v>
       </c>
       <c r="D18" s="16">
@@ -3400,8 +3384,8 @@
       <c r="AO19" s="39" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="41">
-      <c r="A20" s="62" t="n"/>
-      <c r="C20" s="55" t="n">
+      <c r="A20" s="50" t="n"/>
+      <c r="C20" s="15" t="n">
         <v>18</v>
       </c>
       <c r="D20" s="16">
@@ -3533,8 +3517,8 @@
       <c r="AO20" s="39" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="41">
-      <c r="A21" s="62" t="n"/>
-      <c r="C21" s="55" t="n">
+      <c r="A21" s="50" t="n"/>
+      <c r="C21" s="15" t="n">
         <v>19</v>
       </c>
       <c r="D21" s="16">
@@ -3666,7 +3650,7 @@
       <c r="AO21" s="39" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="41">
-      <c r="A22" s="62" t="n"/>
+      <c r="A22" s="50" t="n"/>
       <c r="B22" s="46" t="n"/>
       <c r="C22" s="23" t="n">
         <v>20</v>
@@ -3800,7 +3784,7 @@
       <c r="AO22" s="39" t="n"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="41">
-      <c r="A23" s="62" t="n"/>
+      <c r="A23" s="50" t="n"/>
       <c r="B23" s="47" t="inlineStr">
         <is>
           <t>JS1582</t>
@@ -3938,8 +3922,8 @@
       <c r="AO23" s="39" t="n"/>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="41">
-      <c r="A24" s="62" t="n"/>
-      <c r="C24" s="55" t="n">
+      <c r="A24" s="50" t="n"/>
+      <c r="C24" s="15" t="n">
         <v>22</v>
       </c>
       <c r="D24" s="16">
@@ -4071,8 +4055,8 @@
       <c r="AO24" s="39" t="n"/>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="41">
-      <c r="A25" s="62" t="n"/>
-      <c r="C25" s="55" t="n">
+      <c r="A25" s="50" t="n"/>
+      <c r="C25" s="15" t="n">
         <v>23</v>
       </c>
       <c r="D25" s="16">
@@ -4204,7 +4188,7 @@
       <c r="AO25" s="39" t="n"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="41">
-      <c r="A26" s="62" t="n"/>
+      <c r="A26" s="50" t="n"/>
       <c r="B26" s="46" t="n"/>
       <c r="C26" s="23" t="n">
         <v>24</v>
@@ -4338,7 +4322,7 @@
       <c r="AO26" s="39" t="n"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="41">
-      <c r="A27" s="62" t="n"/>
+      <c r="A27" s="50" t="n"/>
       <c r="B27" s="48" t="inlineStr">
         <is>
           <t>JS1783</t>
@@ -4472,8 +4456,8 @@
       <c r="AO27" s="39" t="n"/>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="41">
-      <c r="A28" s="62" t="n"/>
-      <c r="C28" s="55" t="n">
+      <c r="A28" s="50" t="n"/>
+      <c r="C28" s="15" t="n">
         <v>26</v>
       </c>
       <c r="D28" s="16">
@@ -4601,8 +4585,8 @@
       <c r="AO28" s="39" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="41">
-      <c r="A29" s="62" t="n"/>
-      <c r="C29" s="55" t="n">
+      <c r="A29" s="50" t="n"/>
+      <c r="C29" s="15" t="n">
         <v>27</v>
       </c>
       <c r="D29" s="16">
@@ -4730,7 +4714,7 @@
       <c r="AO29" s="39" t="n"/>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="41">
-      <c r="A30" s="62" t="n"/>
+      <c r="A30" s="50" t="n"/>
       <c r="B30" s="46" t="n"/>
       <c r="C30" s="23" t="n">
         <v>28</v>
@@ -4860,7 +4844,7 @@
       <c r="AO30" s="39" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="41">
-      <c r="A31" s="62" t="n"/>
+      <c r="A31" s="50" t="n"/>
       <c r="B31" s="53" t="inlineStr">
         <is>
           <t>JS1787</t>
@@ -4994,8 +4978,8 @@
       <c r="AO31" s="39" t="n"/>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="41">
-      <c r="A32" s="62" t="n"/>
-      <c r="C32" s="55" t="n">
+      <c r="A32" s="50" t="n"/>
+      <c r="C32" s="15" t="n">
         <v>30</v>
       </c>
       <c r="D32" s="16">
@@ -5123,8 +5107,8 @@
       <c r="AO32" s="39" t="n"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="41">
-      <c r="A33" s="62" t="n"/>
-      <c r="C33" s="55" t="n">
+      <c r="A33" s="50" t="n"/>
+      <c r="C33" s="15" t="n">
         <v>31</v>
       </c>
       <c r="D33" s="16">

</xml_diff>

<commit_message>
Write functionality for outputting to XML and saves counted images - tried adding progress dialog
</commit_message>
<xml_diff>
--- a/Arginine CLS with pH BLOB_DETECTOR.xlsx
+++ b/Arginine CLS with pH BLOB_DETECTOR.xlsx
@@ -1182,7 +1182,9 @@
         <f t="array" ref="S3">Q3*_xlfn.SWITCH(R3, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$3</f>
         <v/>
       </c>
-      <c r="T3" s="12" t="n"/>
+      <c r="T3" s="12" t="n">
+        <v>110</v>
+      </c>
       <c r="U3" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1320,7 +1322,9 @@
         <f t="array" ref="S4">Q4*_xlfn.SWITCH(R4, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$4</f>
         <v/>
       </c>
-      <c r="T4" s="20" t="n"/>
+      <c r="T4" s="20" t="n">
+        <v>131</v>
+      </c>
       <c r="U4" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1458,7 +1462,9 @@
         <f t="array" ref="S5">Q5*_xlfn.SWITCH(R5, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$5</f>
         <v/>
       </c>
-      <c r="T5" s="20" t="n"/>
+      <c r="T5" s="20" t="n">
+        <v>70</v>
+      </c>
       <c r="U5" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1597,7 +1603,9 @@
         <f t="array" ref="S6">Q6*_xlfn.SWITCH(R6, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$6</f>
         <v/>
       </c>
-      <c r="T6" s="28" t="n"/>
+      <c r="T6" s="28" t="n">
+        <v>108</v>
+      </c>
       <c r="U6" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1740,7 +1748,9 @@
         <f t="array" ref="S7">Q7*_xlfn.SWITCH(R7, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$7</f>
         <v/>
       </c>
-      <c r="T7" s="12" t="n"/>
+      <c r="T7" s="12" t="n">
+        <v>188</v>
+      </c>
       <c r="U7" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1878,7 +1888,9 @@
         <f t="array" ref="S8">Q8*_xlfn.SWITCH(R8, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$8</f>
         <v/>
       </c>
-      <c r="T8" s="20" t="n"/>
+      <c r="T8" s="20" t="n">
+        <v>87</v>
+      </c>
       <c r="U8" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2016,7 +2028,9 @@
         <f t="array" ref="S9">Q9*_xlfn.SWITCH(R9, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$9</f>
         <v/>
       </c>
-      <c r="T9" s="20" t="n"/>
+      <c r="T9" s="20" t="n">
+        <v>151</v>
+      </c>
       <c r="U9" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2153,7 +2167,9 @@
         <f t="array" ref="S10">Q10*_xlfn.SWITCH(R10, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$10</f>
         <v/>
       </c>
-      <c r="T10" s="28" t="n"/>
+      <c r="T10" s="28" t="n">
+        <v>206</v>
+      </c>
       <c r="U10" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2296,7 +2312,9 @@
         <f t="array" ref="S11">Q11*_xlfn.SWITCH(R11, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$11</f>
         <v/>
       </c>
-      <c r="T11" s="12" t="n"/>
+      <c r="T11" s="12" t="n">
+        <v>132</v>
+      </c>
       <c r="U11" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2434,7 +2452,9 @@
         <f t="array" ref="S12">Q12*_xlfn.SWITCH(R12, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$12</f>
         <v/>
       </c>
-      <c r="T12" s="20" t="n"/>
+      <c r="T12" s="20" t="n">
+        <v>105</v>
+      </c>
       <c r="U12" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2572,7 +2592,9 @@
         <f t="array" ref="S13">Q13*_xlfn.SWITCH(R13, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$13</f>
         <v/>
       </c>
-      <c r="T13" s="20" t="n"/>
+      <c r="T13" s="20" t="n">
+        <v>132</v>
+      </c>
       <c r="U13" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2711,7 +2733,9 @@
         <f t="array" ref="S14">Q14*_xlfn.SWITCH(R14, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$14</f>
         <v/>
       </c>
-      <c r="T14" s="28" t="n"/>
+      <c r="T14" s="28" t="n">
+        <v>178</v>
+      </c>
       <c r="U14" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2854,7 +2878,9 @@
         <f t="array" ref="S15">Q15*_xlfn.SWITCH(R15, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$15</f>
         <v/>
       </c>
-      <c r="T15" s="12" t="n"/>
+      <c r="T15" s="12" t="n">
+        <v>44</v>
+      </c>
       <c r="U15" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2992,7 +3018,9 @@
         <f t="array" ref="S16">Q16*_xlfn.SWITCH(R16, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$16</f>
         <v/>
       </c>
-      <c r="T16" s="20" t="n"/>
+      <c r="T16" s="20" t="n">
+        <v>204</v>
+      </c>
       <c r="U16" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3130,7 +3158,9 @@
         <f t="array" ref="S17">Q17*_xlfn.SWITCH(R17, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$17</f>
         <v/>
       </c>
-      <c r="T17" s="20" t="n"/>
+      <c r="T17" s="20" t="n">
+        <v>197</v>
+      </c>
       <c r="U17" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3268,7 +3298,9 @@
         <f t="array" ref="S18">Q18*_xlfn.SWITCH(R18, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$18</f>
         <v/>
       </c>
-      <c r="T18" s="20" t="n"/>
+      <c r="T18" s="20" t="n">
+        <v>38</v>
+      </c>
       <c r="U18" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3415,7 +3447,9 @@
         <f t="array" ref="S19">Q19*_xlfn.SWITCH(R19, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$19</f>
         <v/>
       </c>
-      <c r="T19" s="36" t="n"/>
+      <c r="T19" s="36" t="n">
+        <v>82</v>
+      </c>
       <c r="U19" s="37" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3550,7 +3584,9 @@
         <f t="array" ref="S20">Q20*_xlfn.SWITCH(R20, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$20</f>
         <v/>
       </c>
-      <c r="T20" s="20" t="n"/>
+      <c r="T20" s="20" t="n">
+        <v>109</v>
+      </c>
       <c r="U20" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3689,7 +3725,9 @@
         <f t="array" ref="S21">Q21*_xlfn.SWITCH(R21, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$21</f>
         <v/>
       </c>
-      <c r="T21" s="20" t="n"/>
+      <c r="T21" s="20" t="n">
+        <v>96</v>
+      </c>
       <c r="U21" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3829,7 +3867,9 @@
         <f t="array" ref="S22">Q22*_xlfn.SWITCH(R22, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$22</f>
         <v/>
       </c>
-      <c r="T22" s="28" t="n"/>
+      <c r="T22" s="28" t="n">
+        <v>91</v>
+      </c>
       <c r="U22" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3973,7 +4013,9 @@
         <f t="array" ref="S23">Q23*_xlfn.SWITCH(R23, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$23</f>
         <v/>
       </c>
-      <c r="T23" s="12" t="n"/>
+      <c r="T23" s="12" t="n">
+        <v>215</v>
+      </c>
       <c r="U23" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4112,7 +4154,9 @@
         <f t="array" ref="S24">Q24*_xlfn.SWITCH(R24, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$24</f>
         <v/>
       </c>
-      <c r="T24" s="20" t="n"/>
+      <c r="T24" s="20" t="n">
+        <v>206</v>
+      </c>
       <c r="U24" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4251,7 +4295,9 @@
         <f t="array" ref="S25">Q25*_xlfn.SWITCH(R25, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$25</f>
         <v/>
       </c>
-      <c r="T25" s="20" t="n"/>
+      <c r="T25" s="20" t="n">
+        <v>62</v>
+      </c>
       <c r="U25" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4391,7 +4437,9 @@
         <f t="array" ref="S26">Q26*_xlfn.SWITCH(R26, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$26</f>
         <v/>
       </c>
-      <c r="T26" s="28" t="n"/>
+      <c r="T26" s="28" t="n">
+        <v>75</v>
+      </c>
       <c r="U26" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4529,7 +4577,9 @@
         <f t="array" ref="S27">Q27*_xlfn.SWITCH(R27, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$27</f>
         <v/>
       </c>
-      <c r="T27" s="12" t="n"/>
+      <c r="T27" s="12" t="n">
+        <v>125</v>
+      </c>
       <c r="U27" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4662,7 +4712,9 @@
         <f t="array" ref="S28">Q28*_xlfn.SWITCH(R28, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$28</f>
         <v/>
       </c>
-      <c r="T28" s="20" t="n"/>
+      <c r="T28" s="20" t="n">
+        <v>73</v>
+      </c>
       <c r="U28" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4795,7 +4847,9 @@
         <f t="array" ref="S29">Q29*_xlfn.SWITCH(R29, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$29</f>
         <v/>
       </c>
-      <c r="T29" s="20" t="n"/>
+      <c r="T29" s="20" t="n">
+        <v>72</v>
+      </c>
       <c r="U29" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4929,7 +4983,9 @@
         <f t="array" ref="S30">Q30*_xlfn.SWITCH(R30, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$30</f>
         <v/>
       </c>
-      <c r="T30" s="28" t="n"/>
+      <c r="T30" s="28" t="n">
+        <v>61</v>
+      </c>
       <c r="U30" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5067,7 +5123,9 @@
         <f t="array" ref="S31">Q31*_xlfn.SWITCH(R31, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$31</f>
         <v/>
       </c>
-      <c r="T31" s="12" t="n"/>
+      <c r="T31" s="12" t="n">
+        <v>39</v>
+      </c>
       <c r="U31" s="13" t="inlineStr">
         <is>
           <t>x1000</t>
@@ -5200,7 +5258,9 @@
         <f t="array" ref="S32">Q32*_xlfn.SWITCH(R32, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$32</f>
         <v/>
       </c>
-      <c r="T32" s="20" t="n"/>
+      <c r="T32" s="20" t="n">
+        <v>34</v>
+      </c>
       <c r="U32" s="21" t="inlineStr">
         <is>
           <t>x1000</t>
@@ -5339,7 +5399,9 @@
         <f t="array" ref="S33">Q33*_xlfn.SWITCH(R33, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$33</f>
         <v/>
       </c>
-      <c r="T33" s="20" t="n"/>
+      <c r="T33" s="20" t="n">
+        <v>25</v>
+      </c>
       <c r="U33" s="21" t="inlineStr">
         <is>
           <t>x1000</t>
@@ -5479,7 +5541,9 @@
         <f t="array" ref="S34">Q34*_xlfn.SWITCH(R34, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$34</f>
         <v/>
       </c>
-      <c r="T34" s="28" t="n"/>
+      <c r="T34" s="28" t="n">
+        <v>38</v>
+      </c>
       <c r="U34" s="29" t="inlineStr">
         <is>
           <t>x1000</t>
@@ -6547,7 +6611,7 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="F3:F34 I3:I34 L3:L34 O3:O34 R3:R34 U3:U34 X3:X34 AA3:AA34 AD3:AD34 AG3:AG34 AJ3:AJ34 AM3:AM34" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" prompt="Dilution value" type="list">
+    <dataValidation sqref="F3:F34 I3:I34 L3:L34 O3:O34 R3:R34 U3:U34 X3:X34 AA3:AA34 AD3:AD34 AG3:AG34 AJ3:AJ34 AM3:AM34" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="1" prompt="Dilution value" type="list">
       <formula1>"x10,x100,x1000"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Counted colonies for Day 17
</commit_message>
<xml_diff>
--- a/Arginine CLS with pH BLOB_DETECTOR.xlsx
+++ b/Arginine CLS with pH BLOB_DETECTOR.xlsx
@@ -1194,7 +1194,9 @@
         <f t="array" ref="V3">T3*_xlfn.SWITCH(U3, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$3</f>
         <v/>
       </c>
-      <c r="W3" s="9" t="n"/>
+      <c r="W3" s="9" t="n">
+        <v>69</v>
+      </c>
       <c r="X3" s="10" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1334,7 +1336,9 @@
         <f t="array" ref="V4">T4*_xlfn.SWITCH(U4, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$4</f>
         <v/>
       </c>
-      <c r="W4" s="17" t="n"/>
+      <c r="W4" s="17" t="n">
+        <v>103</v>
+      </c>
       <c r="X4" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1474,7 +1478,9 @@
         <f t="array" ref="V5">T5*_xlfn.SWITCH(U5, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$5</f>
         <v/>
       </c>
-      <c r="W5" s="17" t="n"/>
+      <c r="W5" s="17" t="n">
+        <v>95</v>
+      </c>
       <c r="X5" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1615,7 +1621,9 @@
         <f t="array" ref="V6">T6*_xlfn.SWITCH(U6, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$6</f>
         <v/>
       </c>
-      <c r="W6" s="25" t="n"/>
+      <c r="W6" s="25" t="n">
+        <v>101</v>
+      </c>
       <c r="X6" s="26" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1760,7 +1768,9 @@
         <f t="array" ref="V7">T7*_xlfn.SWITCH(U7, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$7</f>
         <v/>
       </c>
-      <c r="W7" s="9" t="n"/>
+      <c r="W7" s="9" t="n">
+        <v>147</v>
+      </c>
       <c r="X7" s="10" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1900,7 +1910,9 @@
         <f t="array" ref="V8">T8*_xlfn.SWITCH(U8, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$8</f>
         <v/>
       </c>
-      <c r="W8" s="17" t="n"/>
+      <c r="W8" s="17" t="n">
+        <v>55</v>
+      </c>
       <c r="X8" s="18" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2040,7 +2052,9 @@
         <f t="array" ref="V9">T9*_xlfn.SWITCH(U9, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$9</f>
         <v/>
       </c>
-      <c r="W9" s="17" t="n"/>
+      <c r="W9" s="17" t="n">
+        <v>101</v>
+      </c>
       <c r="X9" s="18" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2179,7 +2193,9 @@
         <f t="array" ref="V10">T10*_xlfn.SWITCH(U10, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$10</f>
         <v/>
       </c>
-      <c r="W10" s="25" t="n"/>
+      <c r="W10" s="25" t="n">
+        <v>81</v>
+      </c>
       <c r="X10" s="26" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2324,7 +2340,9 @@
         <f t="array" ref="V11">T11*_xlfn.SWITCH(U11, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$11</f>
         <v/>
       </c>
-      <c r="W11" s="9" t="n"/>
+      <c r="W11" s="9" t="n">
+        <v>65</v>
+      </c>
       <c r="X11" s="10" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2464,7 +2482,9 @@
         <f t="array" ref="V12">T12*_xlfn.SWITCH(U12, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$12</f>
         <v/>
       </c>
-      <c r="W12" s="17" t="n"/>
+      <c r="W12" s="17" t="n">
+        <v>32</v>
+      </c>
       <c r="X12" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2604,7 +2624,9 @@
         <f t="array" ref="V13">T13*_xlfn.SWITCH(U13, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$13</f>
         <v/>
       </c>
-      <c r="W13" s="17" t="n"/>
+      <c r="W13" s="17" t="n">
+        <v>59</v>
+      </c>
       <c r="X13" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2745,7 +2767,9 @@
         <f t="array" ref="V14">T14*_xlfn.SWITCH(U14, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$14</f>
         <v/>
       </c>
-      <c r="W14" s="25" t="n"/>
+      <c r="W14" s="25" t="n">
+        <v>66</v>
+      </c>
       <c r="X14" s="26" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2890,7 +2914,9 @@
         <f t="array" ref="V15">T15*_xlfn.SWITCH(U15, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$15</f>
         <v/>
       </c>
-      <c r="W15" s="9" t="n"/>
+      <c r="W15" s="9" t="n">
+        <v>18</v>
+      </c>
       <c r="X15" s="10" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3030,7 +3056,9 @@
         <f t="array" ref="V16">T16*_xlfn.SWITCH(U16, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$16</f>
         <v/>
       </c>
-      <c r="W16" s="17" t="n"/>
+      <c r="W16" s="17" t="n">
+        <v>62</v>
+      </c>
       <c r="X16" s="18" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3170,7 +3198,9 @@
         <f t="array" ref="V17">T17*_xlfn.SWITCH(U17, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$17</f>
         <v/>
       </c>
-      <c r="W17" s="17" t="n"/>
+      <c r="W17" s="17" t="n">
+        <v>112</v>
+      </c>
       <c r="X17" s="18" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3310,7 +3340,9 @@
         <f t="array" ref="V18">T18*_xlfn.SWITCH(U18, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$18</f>
         <v/>
       </c>
-      <c r="W18" s="17" t="n"/>
+      <c r="W18" s="17" t="n">
+        <v>30</v>
+      </c>
       <c r="X18" s="18" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3459,7 +3491,9 @@
         <f t="array" ref="V19">T19*_xlfn.SWITCH(U19, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$19</f>
         <v/>
       </c>
-      <c r="W19" s="33" t="n"/>
+      <c r="W19" s="33" t="n">
+        <v>84</v>
+      </c>
       <c r="X19" s="34" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3596,7 +3630,9 @@
         <f t="array" ref="V20">T20*_xlfn.SWITCH(U20, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$20</f>
         <v/>
       </c>
-      <c r="W20" s="17" t="n"/>
+      <c r="W20" s="17" t="n">
+        <v>55</v>
+      </c>
       <c r="X20" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3737,7 +3773,9 @@
         <f t="array" ref="V21">T21*_xlfn.SWITCH(U21, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$21</f>
         <v/>
       </c>
-      <c r="W21" s="17" t="n"/>
+      <c r="W21" s="17" t="n">
+        <v>71</v>
+      </c>
       <c r="X21" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3879,7 +3917,9 @@
         <f t="array" ref="V22">T22*_xlfn.SWITCH(U22, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$22</f>
         <v/>
       </c>
-      <c r="W22" s="25" t="n"/>
+      <c r="W22" s="25" t="n">
+        <v>56</v>
+      </c>
       <c r="X22" s="26" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4025,7 +4065,9 @@
         <f t="array" ref="V23">T23*_xlfn.SWITCH(U23, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$23</f>
         <v/>
       </c>
-      <c r="W23" s="9" t="n"/>
+      <c r="W23" s="9" t="n">
+        <v>165</v>
+      </c>
       <c r="X23" s="10" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4166,7 +4208,9 @@
         <f t="array" ref="V24">T24*_xlfn.SWITCH(U24, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$24</f>
         <v/>
       </c>
-      <c r="W24" s="17" t="n"/>
+      <c r="W24" s="17" t="n">
+        <v>183</v>
+      </c>
       <c r="X24" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4307,7 +4351,9 @@
         <f t="array" ref="V25">T25*_xlfn.SWITCH(U25, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$25</f>
         <v/>
       </c>
-      <c r="W25" s="17" t="n"/>
+      <c r="W25" s="17" t="n">
+        <v>93</v>
+      </c>
       <c r="X25" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4449,7 +4495,9 @@
         <f t="array" ref="V26">T26*_xlfn.SWITCH(U26, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$26</f>
         <v/>
       </c>
-      <c r="W26" s="25" t="n"/>
+      <c r="W26" s="25" t="n">
+        <v>95</v>
+      </c>
       <c r="X26" s="26" t="inlineStr">
         <is>
           <t>x10</t>
@@ -4589,7 +4637,9 @@
         <f t="array" ref="V27">T27*_xlfn.SWITCH(U27, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$27</f>
         <v/>
       </c>
-      <c r="W27" s="9" t="n"/>
+      <c r="W27" s="9" t="n">
+        <v>54</v>
+      </c>
       <c r="X27" s="10" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4724,7 +4774,9 @@
         <f t="array" ref="V28">T28*_xlfn.SWITCH(U28, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$28</f>
         <v/>
       </c>
-      <c r="W28" s="17" t="n"/>
+      <c r="W28" s="17" t="n">
+        <v>42</v>
+      </c>
       <c r="X28" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4859,7 +4911,9 @@
         <f t="array" ref="V29">T29*_xlfn.SWITCH(U29, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$29</f>
         <v/>
       </c>
-      <c r="W29" s="17" t="n"/>
+      <c r="W29" s="17" t="n">
+        <v>59</v>
+      </c>
       <c r="X29" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4995,7 +5049,9 @@
         <f t="array" ref="V30">T30*_xlfn.SWITCH(U30, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$30</f>
         <v/>
       </c>
-      <c r="W30" s="25" t="n"/>
+      <c r="W30" s="25" t="n">
+        <v>48</v>
+      </c>
       <c r="X30" s="26" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5135,7 +5191,9 @@
         <f t="array" ref="V31">T31*_xlfn.SWITCH(U31, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$31</f>
         <v/>
       </c>
-      <c r="W31" s="9" t="n"/>
+      <c r="W31" s="9" t="n">
+        <v>184</v>
+      </c>
       <c r="X31" s="10" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5270,7 +5328,9 @@
         <f t="array" ref="V32">T32*_xlfn.SWITCH(U32, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$32</f>
         <v/>
       </c>
-      <c r="W32" s="17" t="n"/>
+      <c r="W32" s="17" t="n">
+        <v>138</v>
+      </c>
       <c r="X32" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5411,7 +5471,9 @@
         <f t="array" ref="V33">T33*_xlfn.SWITCH(U33, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$33</f>
         <v/>
       </c>
-      <c r="W33" s="17" t="n"/>
+      <c r="W33" s="17" t="n">
+        <v>138</v>
+      </c>
       <c r="X33" s="18" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5553,7 +5615,9 @@
         <f t="array" ref="V34">T34*_xlfn.SWITCH(U34, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$34</f>
         <v/>
       </c>
-      <c r="W34" s="25" t="n"/>
+      <c r="W34" s="25" t="n">
+        <v>60</v>
+      </c>
       <c r="X34" s="26" t="inlineStr">
         <is>
           <t>x100</t>

</xml_diff>

<commit_message>
Counted colonies for Day 19
</commit_message>
<xml_diff>
--- a/Arginine CLS with pH BLOB_DETECTOR.xlsx
+++ b/Arginine CLS with pH BLOB_DETECTOR.xlsx
@@ -1206,7 +1206,9 @@
         <f t="array" ref="Y3">W3*_xlfn.SWITCH(X3, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$3</f>
         <v/>
       </c>
-      <c r="Z3" s="12" t="n"/>
+      <c r="Z3" s="12" t="n">
+        <v>37</v>
+      </c>
       <c r="AA3" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1348,7 +1350,9 @@
         <f t="array" ref="Y4">W4*_xlfn.SWITCH(X4, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$4</f>
         <v/>
       </c>
-      <c r="Z4" s="20" t="n"/>
+      <c r="Z4" s="20" t="n">
+        <v>37</v>
+      </c>
       <c r="AA4" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1490,7 +1494,9 @@
         <f t="array" ref="Y5">W5*_xlfn.SWITCH(X5, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$5</f>
         <v/>
       </c>
-      <c r="Z5" s="20" t="n"/>
+      <c r="Z5" s="20" t="n">
+        <v>44</v>
+      </c>
       <c r="AA5" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1633,7 +1639,9 @@
         <f t="array" ref="Y6">W6*_xlfn.SWITCH(X6, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$6</f>
         <v/>
       </c>
-      <c r="Z6" s="28" t="n"/>
+      <c r="Z6" s="28" t="n">
+        <v>34</v>
+      </c>
       <c r="AA6" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -1780,7 +1788,9 @@
         <f t="array" ref="Y7">W7*_xlfn.SWITCH(X7, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$7</f>
         <v/>
       </c>
-      <c r="Z7" s="12" t="n"/>
+      <c r="Z7" s="12" t="n">
+        <v>106</v>
+      </c>
       <c r="AA7" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1922,7 +1932,9 @@
         <f t="array" ref="Y8">W8*_xlfn.SWITCH(X8, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$8</f>
         <v/>
       </c>
-      <c r="Z8" s="20" t="n"/>
+      <c r="Z8" s="20" t="n">
+        <v>34</v>
+      </c>
       <c r="AA8" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2064,7 +2076,9 @@
         <f t="array" ref="Y9">W9*_xlfn.SWITCH(X9, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$9</f>
         <v/>
       </c>
-      <c r="Z9" s="20" t="n"/>
+      <c r="Z9" s="20" t="n">
+        <v>48</v>
+      </c>
       <c r="AA9" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2205,7 +2219,9 @@
         <f t="array" ref="Y10">W10*_xlfn.SWITCH(X10, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$10</f>
         <v/>
       </c>
-      <c r="Z10" s="28" t="n"/>
+      <c r="Z10" s="28" t="n">
+        <v>312</v>
+      </c>
       <c r="AA10" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2352,7 +2368,9 @@
         <f t="array" ref="Y11">W11*_xlfn.SWITCH(X11, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$11</f>
         <v/>
       </c>
-      <c r="Z11" s="12" t="n"/>
+      <c r="Z11" s="12" t="n">
+        <v>59</v>
+      </c>
       <c r="AA11" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2494,7 +2512,9 @@
         <f t="array" ref="Y12">W12*_xlfn.SWITCH(X12, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$12</f>
         <v/>
       </c>
-      <c r="Z12" s="20" t="n"/>
+      <c r="Z12" s="20" t="n">
+        <v>35</v>
+      </c>
       <c r="AA12" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2636,7 +2656,9 @@
         <f t="array" ref="Y13">W13*_xlfn.SWITCH(X13, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$13</f>
         <v/>
       </c>
-      <c r="Z13" s="20" t="n"/>
+      <c r="Z13" s="20" t="n">
+        <v>72</v>
+      </c>
       <c r="AA13" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2779,7 +2801,9 @@
         <f t="array" ref="Y14">W14*_xlfn.SWITCH(X14, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$14</f>
         <v/>
       </c>
-      <c r="Z14" s="28" t="n"/>
+      <c r="Z14" s="28" t="n">
+        <v>69</v>
+      </c>
       <c r="AA14" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -2926,7 +2950,9 @@
         <f t="array" ref="Y15">W15*_xlfn.SWITCH(X15, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$15</f>
         <v/>
       </c>
-      <c r="Z15" s="12" t="n"/>
+      <c r="Z15" s="12" t="n">
+        <v>6</v>
+      </c>
       <c r="AA15" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3068,7 +3094,9 @@
         <f t="array" ref="Y16">W16*_xlfn.SWITCH(X16, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$16</f>
         <v/>
       </c>
-      <c r="Z16" s="20" t="n"/>
+      <c r="Z16" s="20" t="n">
+        <v>32</v>
+      </c>
       <c r="AA16" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3210,7 +3238,9 @@
         <f t="array" ref="Y17">W17*_xlfn.SWITCH(X17, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$17</f>
         <v/>
       </c>
-      <c r="Z17" s="20" t="n"/>
+      <c r="Z17" s="20" t="n">
+        <v>44</v>
+      </c>
       <c r="AA17" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3352,7 +3382,9 @@
         <f t="array" ref="Y18">W18*_xlfn.SWITCH(X18, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$18</f>
         <v/>
       </c>
-      <c r="Z18" s="20" t="n"/>
+      <c r="Z18" s="20" t="n">
+        <v>27</v>
+      </c>
       <c r="AA18" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3503,7 +3535,9 @@
         <f t="array" ref="Y19">W19*_xlfn.SWITCH(X19, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$19</f>
         <v/>
       </c>
-      <c r="Z19" s="36" t="n"/>
+      <c r="Z19" s="36" t="n">
+        <v>79</v>
+      </c>
       <c r="AA19" s="37" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3642,7 +3676,9 @@
         <f t="array" ref="Y20">W20*_xlfn.SWITCH(X20, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$20</f>
         <v/>
       </c>
-      <c r="Z20" s="20" t="n"/>
+      <c r="Z20" s="20" t="n">
+        <v>50</v>
+      </c>
       <c r="AA20" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3785,7 +3821,9 @@
         <f t="array" ref="Y21">W21*_xlfn.SWITCH(X21, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$21</f>
         <v/>
       </c>
-      <c r="Z21" s="20" t="n"/>
+      <c r="Z21" s="20" t="n">
+        <v>51</v>
+      </c>
       <c r="AA21" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3929,7 +3967,9 @@
         <f t="array" ref="Y22">W22*_xlfn.SWITCH(X22, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$22</f>
         <v/>
       </c>
-      <c r="Z22" s="28" t="n"/>
+      <c r="Z22" s="28" t="n">
+        <v>47</v>
+      </c>
       <c r="AA22" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4077,7 +4117,9 @@
         <f t="array" ref="Y23">W23*_xlfn.SWITCH(X23, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$23</f>
         <v/>
       </c>
-      <c r="Z23" s="12" t="n"/>
+      <c r="Z23" s="12" t="n">
+        <v>171</v>
+      </c>
       <c r="AA23" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4220,7 +4262,9 @@
         <f t="array" ref="Y24">W24*_xlfn.SWITCH(X24, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$24</f>
         <v/>
       </c>
-      <c r="Z24" s="20" t="n"/>
+      <c r="Z24" s="20" t="n">
+        <v>165</v>
+      </c>
       <c r="AA24" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4363,7 +4407,9 @@
         <f t="array" ref="Y25">W25*_xlfn.SWITCH(X25, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$25</f>
         <v/>
       </c>
-      <c r="Z25" s="20" t="n"/>
+      <c r="Z25" s="20" t="n">
+        <v>98</v>
+      </c>
       <c r="AA25" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4507,7 +4553,9 @@
         <f t="array" ref="Y26">W26*_xlfn.SWITCH(X26, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$26</f>
         <v/>
       </c>
-      <c r="Z26" s="28" t="n"/>
+      <c r="Z26" s="28" t="n">
+        <v>63</v>
+      </c>
       <c r="AA26" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -4649,7 +4697,9 @@
         <f t="array" ref="Y27">W27*_xlfn.SWITCH(X27, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$27</f>
         <v/>
       </c>
-      <c r="Z27" s="12" t="n"/>
+      <c r="Z27" s="12" t="n">
+        <v>48</v>
+      </c>
       <c r="AA27" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4786,7 +4836,9 @@
         <f t="array" ref="Y28">W28*_xlfn.SWITCH(X28, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$28</f>
         <v/>
       </c>
-      <c r="Z28" s="20" t="n"/>
+      <c r="Z28" s="20" t="n">
+        <v>24</v>
+      </c>
       <c r="AA28" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4923,7 +4975,9 @@
         <f t="array" ref="Y29">W29*_xlfn.SWITCH(X29, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$29</f>
         <v/>
       </c>
-      <c r="Z29" s="20" t="n"/>
+      <c r="Z29" s="20" t="n">
+        <v>53</v>
+      </c>
       <c r="AA29" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5061,7 +5115,9 @@
         <f t="array" ref="Y30">W30*_xlfn.SWITCH(X30, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$30</f>
         <v/>
       </c>
-      <c r="Z30" s="28" t="n"/>
+      <c r="Z30" s="28" t="n">
+        <v>38</v>
+      </c>
       <c r="AA30" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5203,7 +5259,9 @@
         <f t="array" ref="Y31">W31*_xlfn.SWITCH(X31, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$31</f>
         <v/>
       </c>
-      <c r="Z31" s="12" t="n"/>
+      <c r="Z31" s="12" t="n">
+        <v>28</v>
+      </c>
       <c r="AA31" s="13" t="inlineStr">
         <is>
           <t>x1000</t>
@@ -5340,7 +5398,9 @@
         <f t="array" ref="Y32">W32*_xlfn.SWITCH(X32, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$32</f>
         <v/>
       </c>
-      <c r="Z32" s="20" t="n"/>
+      <c r="Z32" s="20" t="n">
+        <v>159</v>
+      </c>
       <c r="AA32" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5483,7 +5543,9 @@
         <f t="array" ref="Y33">W33*_xlfn.SWITCH(X33, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$33</f>
         <v/>
       </c>
-      <c r="Z33" s="20" t="n"/>
+      <c r="Z33" s="20" t="n">
+        <v>60</v>
+      </c>
       <c r="AA33" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -5627,7 +5689,9 @@
         <f t="array" ref="Y34">W34*_xlfn.SWITCH(X34, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$34</f>
         <v/>
       </c>
-      <c r="Z34" s="28" t="n"/>
+      <c r="Z34" s="28" t="n">
+        <v>35</v>
+      </c>
       <c r="AA34" s="29" t="inlineStr">
         <is>
           <t>x100</t>

</xml_diff>

<commit_message>
Solve infinite recursion bug
</commit_message>
<xml_diff>
--- a/Arginine CLS with pH BLOB_DETECTOR.xlsx
+++ b/Arginine CLS with pH BLOB_DETECTOR.xlsx
@@ -1228,7 +1228,9 @@
         <f t="array" ref="AE3">AC3*_xlfn.SWITCH(AD3, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$3</f>
         <v/>
       </c>
-      <c r="AF3" s="12" t="n"/>
+      <c r="AF3" s="12" t="n">
+        <v>80</v>
+      </c>
       <c r="AG3" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1372,7 +1374,9 @@
         <f t="array" ref="AE4">AC4*_xlfn.SWITCH(AD4, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$4</f>
         <v/>
       </c>
-      <c r="AF4" s="20" t="n"/>
+      <c r="AF4" s="20" t="n">
+        <v>70</v>
+      </c>
       <c r="AG4" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1516,7 +1520,9 @@
         <f t="array" ref="AE5">AC5*_xlfn.SWITCH(AD5, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$5</f>
         <v/>
       </c>
-      <c r="AF5" s="20" t="n"/>
+      <c r="AF5" s="20" t="n">
+        <v>43</v>
+      </c>
       <c r="AG5" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1661,7 +1667,9 @@
         <f t="array" ref="AE6">AC6*_xlfn.SWITCH(AD6, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$6</f>
         <v/>
       </c>
-      <c r="AF6" s="28" t="n"/>
+      <c r="AF6" s="28" t="n">
+        <v>176</v>
+      </c>
       <c r="AG6" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1810,7 +1818,9 @@
         <f t="array" ref="AE7">AC7*_xlfn.SWITCH(AD7, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$7</f>
         <v/>
       </c>
-      <c r="AF7" s="12" t="n"/>
+      <c r="AF7" s="12" t="n">
+        <v>7</v>
+      </c>
       <c r="AG7" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -1954,7 +1964,9 @@
         <f t="array" ref="AE8">AC8*_xlfn.SWITCH(AD8, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$8</f>
         <v/>
       </c>
-      <c r="AF8" s="20" t="n"/>
+      <c r="AF8" s="20" t="n">
+        <v>8</v>
+      </c>
       <c r="AG8" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2098,7 +2110,9 @@
         <f t="array" ref="AE9">AC9*_xlfn.SWITCH(AD9, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$9</f>
         <v/>
       </c>
-      <c r="AF9" s="20" t="n"/>
+      <c r="AF9" s="20" t="n">
+        <v>12</v>
+      </c>
       <c r="AG9" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2241,7 +2255,9 @@
         <f t="array" ref="AE10">AC10*_xlfn.SWITCH(AD10, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$10</f>
         <v/>
       </c>
-      <c r="AF10" s="28" t="n"/>
+      <c r="AF10" s="28" t="n">
+        <v>4</v>
+      </c>
       <c r="AG10" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2390,7 +2406,9 @@
         <f t="array" ref="AE11">AC11*_xlfn.SWITCH(AD11, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$11</f>
         <v/>
       </c>
-      <c r="AF11" s="12" t="n"/>
+      <c r="AF11" s="12" t="n">
+        <v>73</v>
+      </c>
       <c r="AG11" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2534,7 +2552,9 @@
         <f t="array" ref="AE12">AC12*_xlfn.SWITCH(AD12, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$12</f>
         <v/>
       </c>
-      <c r="AF12" s="20" t="n"/>
+      <c r="AF12" s="20" t="n">
+        <v>11</v>
+      </c>
       <c r="AG12" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2678,7 +2698,9 @@
         <f t="array" ref="AE13">AC13*_xlfn.SWITCH(AD13, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$13</f>
         <v/>
       </c>
-      <c r="AF13" s="20" t="n"/>
+      <c r="AF13" s="20" t="n">
+        <v>76</v>
+      </c>
       <c r="AG13" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2823,7 +2845,9 @@
         <f t="array" ref="AE14">AC14*_xlfn.SWITCH(AD14, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$14</f>
         <v/>
       </c>
-      <c r="AF14" s="28" t="n"/>
+      <c r="AF14" s="28" t="n">
+        <v>91</v>
+      </c>
       <c r="AG14" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -2972,7 +2996,9 @@
         <f t="array" ref="AE15">AC15*_xlfn.SWITCH(AD15, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$15</f>
         <v/>
       </c>
-      <c r="AF15" s="12" t="n"/>
+      <c r="AF15" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AG15" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3116,7 +3142,9 @@
         <f t="array" ref="AE16">AC16*_xlfn.SWITCH(AD16, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$16</f>
         <v/>
       </c>
-      <c r="AF16" s="20" t="n"/>
+      <c r="AF16" s="20" t="n">
+        <v>4</v>
+      </c>
       <c r="AG16" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3260,7 +3288,9 @@
         <f t="array" ref="AE17">AC17*_xlfn.SWITCH(AD17, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$17</f>
         <v/>
       </c>
-      <c r="AF17" s="20" t="n"/>
+      <c r="AF17" s="20" t="n">
+        <v>4</v>
+      </c>
       <c r="AG17" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3404,7 +3434,9 @@
         <f t="array" ref="AE18">AC18*_xlfn.SWITCH(AD18, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$18</f>
         <v/>
       </c>
-      <c r="AF18" s="20" t="n"/>
+      <c r="AF18" s="20" t="n">
+        <v>4</v>
+      </c>
       <c r="AG18" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3557,7 +3589,9 @@
         <f t="array" ref="AE19">AC19*_xlfn.SWITCH(AD19, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$19</f>
         <v/>
       </c>
-      <c r="AF19" s="36" t="n"/>
+      <c r="AF19" s="36" t="n">
+        <v>31</v>
+      </c>
       <c r="AG19" s="37" t="inlineStr">
         <is>
           <t>x100</t>
@@ -3698,7 +3732,9 @@
         <f t="array" ref="AE20">AC20*_xlfn.SWITCH(AD20, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$20</f>
         <v/>
       </c>
-      <c r="AF20" s="20" t="n"/>
+      <c r="AF20" s="20" t="n">
+        <v>112</v>
+      </c>
       <c r="AG20" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3843,7 +3879,9 @@
         <f t="array" ref="AE21">AC21*_xlfn.SWITCH(AD21, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$21</f>
         <v/>
       </c>
-      <c r="AF21" s="20" t="n"/>
+      <c r="AF21" s="20" t="n">
+        <v>220</v>
+      </c>
       <c r="AG21" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -3989,7 +4027,9 @@
         <f t="array" ref="AE22">AC22*_xlfn.SWITCH(AD22, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$22</f>
         <v/>
       </c>
-      <c r="AF22" s="28" t="n"/>
+      <c r="AF22" s="28" t="n">
+        <v>57</v>
+      </c>
       <c r="AG22" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -4139,7 +4179,9 @@
         <f t="array" ref="AE23">AC23*_xlfn.SWITCH(AD23, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$23</f>
         <v/>
       </c>
-      <c r="AF23" s="12" t="n"/>
+      <c r="AF23" s="12" t="n">
+        <v>105</v>
+      </c>
       <c r="AG23" s="13" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4284,7 +4326,9 @@
         <f t="array" ref="AE24">AC24*_xlfn.SWITCH(AD24, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$24</f>
         <v/>
       </c>
-      <c r="AF24" s="20" t="n"/>
+      <c r="AF24" s="20" t="n">
+        <v>60</v>
+      </c>
       <c r="AG24" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4429,7 +4473,9 @@
         <f t="array" ref="AE25">AC25*_xlfn.SWITCH(AD25, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$25</f>
         <v/>
       </c>
-      <c r="AF25" s="20" t="n"/>
+      <c r="AF25" s="20" t="n">
+        <v>133</v>
+      </c>
       <c r="AG25" s="21" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4575,7 +4621,9 @@
         <f t="array" ref="AE26">AC26*_xlfn.SWITCH(AD26, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$26</f>
         <v/>
       </c>
-      <c r="AF26" s="28" t="n"/>
+      <c r="AF26" s="28" t="n">
+        <v>180</v>
+      </c>
       <c r="AG26" s="29" t="inlineStr">
         <is>
           <t>x100</t>
@@ -4719,7 +4767,9 @@
         <f t="array" ref="AE27">AC27*_xlfn.SWITCH(AD27, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$27</f>
         <v/>
       </c>
-      <c r="AF27" s="12" t="n"/>
+      <c r="AF27" s="12" t="n">
+        <v>251</v>
+      </c>
       <c r="AG27" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -4858,7 +4908,9 @@
         <f t="array" ref="AE28">AC28*_xlfn.SWITCH(AD28, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$28</f>
         <v/>
       </c>
-      <c r="AF28" s="20" t="n"/>
+      <c r="AF28" s="20" t="n">
+        <v>252</v>
+      </c>
       <c r="AG28" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -4997,7 +5049,9 @@
         <f t="array" ref="AE29">AC29*_xlfn.SWITCH(AD29, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$29</f>
         <v/>
       </c>
-      <c r="AF29" s="20" t="n"/>
+      <c r="AF29" s="20" t="n">
+        <v>251</v>
+      </c>
       <c r="AG29" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -5137,7 +5191,9 @@
         <f t="array" ref="AE30">AC30*_xlfn.SWITCH(AD30, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$30</f>
         <v/>
       </c>
-      <c r="AF30" s="28" t="n"/>
+      <c r="AF30" s="28" t="n">
+        <v>223</v>
+      </c>
       <c r="AG30" s="29" t="inlineStr">
         <is>
           <t>x10</t>
@@ -5281,7 +5337,9 @@
         <f t="array" ref="AE31">AC31*_xlfn.SWITCH(AD31, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$31</f>
         <v/>
       </c>
-      <c r="AF31" s="12" t="n"/>
+      <c r="AF31" s="12" t="n">
+        <v>180</v>
+      </c>
       <c r="AG31" s="13" t="inlineStr">
         <is>
           <t>x10</t>
@@ -5420,7 +5478,9 @@
         <f t="array" ref="AE32">AC32*_xlfn.SWITCH(AD32, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$32</f>
         <v/>
       </c>
-      <c r="AF32" s="20" t="n"/>
+      <c r="AF32" s="20" t="n">
+        <v>245</v>
+      </c>
       <c r="AG32" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -5565,7 +5625,9 @@
         <f t="array" ref="AE33">AC33*_xlfn.SWITCH(AD33, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$33</f>
         <v/>
       </c>
-      <c r="AF33" s="20" t="n"/>
+      <c r="AF33" s="20" t="n">
+        <v>67</v>
+      </c>
       <c r="AG33" s="21" t="inlineStr">
         <is>
           <t>x10</t>
@@ -5711,7 +5773,9 @@
         <f t="array" ref="AE34">AC34*_xlfn.SWITCH(AD34, "x10", 0.01, "x100", 0.1,"x1000", 1, 0)/$D$34</f>
         <v/>
       </c>
-      <c r="AF34" s="28" t="n"/>
+      <c r="AF34" s="28" t="n">
+        <v>10</v>
+      </c>
       <c r="AG34" s="29" t="inlineStr">
         <is>
           <t>x10</t>

</xml_diff>